<commit_message>
Updated the excel macro to attach a word file to first page of excel sheet.
</commit_message>
<xml_diff>
--- a/bccsu/reports/templates/template.xlsx
+++ b/bccsu/reports/templates/template.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\Documents\Projects\bccsu-tools\bccsu\reports\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C98114-0047-4D78-BDEC-996D54477D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83004BE-6414-402E-832A-CD35645C19B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Request" sheetId="41" r:id="rId1"/>
+    <sheet name="Request" sheetId="42" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk503950932" localSheetId="0">Request!#REF!</definedName>
-    <definedName name="all">Request!#REF!</definedName>
+    <definedName name="all">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -251,11 +250,8 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -425,19 +421,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CF33C2-40E8-4BFA-B351-887890A98467}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C5" s="1"/>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>